<commit_message>
emailReports function is added in scripts class
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -58,64 +58,49 @@
     <t xml:space="preserve">search</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing Error page2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“7”</t>
+    <t xml:space="preserve">Product Listing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“3”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productCatalogPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productDetailPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking Filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“4”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applyFilters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COD Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“5”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emailing Reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“10”</t>
   </si>
   <si>
     <t xml:space="preserve">YES</t>
   </si>
   <si>
-    <t xml:space="preserve">test2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testErrorpage1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“3”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productCatalogPage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productDetailPage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checking Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“4”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applyFilters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COD Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“5”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clearCart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cartCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Error page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“6”</t>
+    <t xml:space="preserve">emailReport</t>
   </si>
 </sst>
 </file>
@@ -249,23 +234,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,132 +305,75 @@
       <c r="B4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
+      <c r="I6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
emailReport functionsends eports from tab@styletag.com and added report's file_name variable in ExcelWrite file
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">“2”</t>
   </si>
   <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">search</t>
   </si>
   <si>
@@ -95,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">“10”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
   </si>
   <si>
     <t xml:space="preserve">emailReport</t>
@@ -234,22 +234,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,54 +292,54 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>7</v>
@@ -347,30 +348,27 @@
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
added writig to reports in all functions of script class
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -237,7 +237,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -342,7 +342,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
login function - added tescases, TestSuit.xls has proper test case IDS
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Log In</t>
   </si>
   <si>
-    <t xml:space="preserve">“1”</t>
+    <t xml:space="preserve">“1434”</t>
   </si>
   <si>
     <t xml:space="preserve">NO</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Search Page</t>
   </si>
   <si>
-    <t xml:space="preserve">“2”</t>
+    <t xml:space="preserve">“161 162 45”</t>
   </si>
   <si>
     <t xml:space="preserve">YES</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Product Listing</t>
   </si>
   <si>
-    <t xml:space="preserve">“3”</t>
+    <t xml:space="preserve">“431 53 551 561 562”</t>
   </si>
   <si>
     <t xml:space="preserve">productCatalogPage</t>
@@ -73,31 +73,33 @@
     <t xml:space="preserve">productDetailPage</t>
   </si>
   <si>
+    <t xml:space="preserve">COD Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“1434 431 53 551 561 562 
+612 8121 8123 8225 8471 8472 911”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkout</t>
+  </si>
+  <si>
     <t xml:space="preserve">Checking Filters</t>
   </si>
   <si>
-    <t xml:space="preserve">“4”</t>
+    <t xml:space="preserve">“431 441 442 443 444 445 446
+447 448 45”</t>
   </si>
   <si>
     <t xml:space="preserve">applyFilters</t>
   </si>
   <si>
-    <t xml:space="preserve">COD Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“5”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cartCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkout</t>
-  </si>
-  <si>
     <t xml:space="preserve">Emailing Reports</t>
   </si>
   <si>
-    <t xml:space="preserve">“10”</t>
+    <t xml:space="preserve">“007”</t>
   </si>
   <si>
     <t xml:space="preserve">emailReport</t>
@@ -196,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +217,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -237,20 +243,20 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.9540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,46 +323,46 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new function clearCartItems- which clears all items in the cart
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -49,7 +49,10 @@
     <t xml:space="preserve">login</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing</t>
+    <t xml:space="preserve">Multi line items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“ ”</t>
   </si>
   <si>
     <t xml:space="preserve">YES</t>
@@ -61,22 +64,25 @@
     <t xml:space="preserve">productDetailPage</t>
   </si>
   <si>
+    <t xml:space="preserve">clearCartItems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“161 162 45”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Listing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“431 53 551 561 562”</t>
+  </si>
+  <si>
     <t xml:space="preserve">cartCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“161 162 45”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“431 53 551 561 562”</t>
   </si>
   <si>
     <t xml:space="preserve">COD Order</t>
@@ -114,7 +120,7 @@
     <t xml:space="preserve">filters in test</t>
   </si>
   <si>
-    <t xml:space="preserve">“ ”</t>
+    <t xml:space="preserve">checking cartitemclear</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -165,6 +171,13 @@
       <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -210,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +241,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,24 +269,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.83163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,85 +324,82 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>7</v>
@@ -394,64 +408,75 @@
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checkout with order-review modified
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">confirmationPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkingconfirmation page</t>
   </si>
 </sst>
 </file>
@@ -275,23 +278,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,16 +494,54 @@
       <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="L10" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new checkoutLogin()- which login at checkout/email page
</commit_message>
<xml_diff>
--- a/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/src/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Action2</t>
   </si>
   <si>
-    <t xml:space="preserve">Log In</t>
+    <t xml:space="preserve">Login at Home page</t>
   </si>
   <si>
     <t xml:space="preserve">“1434”</t>
@@ -49,47 +49,68 @@
     <t xml:space="preserve">login</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi line items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“ 431 53”</t>
+    <t xml:space="preserve">logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login at product Listing page</t>
   </si>
   <si>
     <t xml:space="preserve">productCatalogPage</t>
   </si>
   <si>
+    <t xml:space="preserve">Login at Product detail Page</t>
+  </si>
+  <si>
     <t xml:space="preserve">productDetailPage</t>
   </si>
   <si>
+    <t xml:space="preserve">Login at checkout page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkoutLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login in search page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“161 162 45”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding multple products from listing page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“431 53 551 561 562”</t>
+  </si>
+  <si>
     <t xml:space="preserve">cartCheck</t>
   </si>
   <si>
-    <t xml:space="preserve">Search Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“161 162 45”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“431 53 551 561 562”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COD Order</t>
+    <t xml:space="preserve">clearCartItems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding product from search page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placing COD order</t>
   </si>
   <si>
     <t xml:space="preserve">“1434 431 53 551 561 562 
 612 8121 8123 8225 8471 8472 911”</t>
   </si>
   <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">checkout</t>
   </si>
   <si>
     <t xml:space="preserve">orderCOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmationPage</t>
   </si>
   <si>
     <t xml:space="preserve">Checking Filters</t>
@@ -123,13 +144,13 @@
     <t xml:space="preserve">“”</t>
   </si>
   <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmationPage</t>
-  </si>
-  <si>
     <t xml:space="preserve">checkingconfirmation page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi line items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“ 431 53”</t>
   </si>
 </sst>
 </file>
@@ -253,12 +274,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -278,23 +299,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.9438775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.6122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,222 +354,351 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="2"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="3"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="2"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="3"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="2"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="3"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="2"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="K7" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>34</v>
+      <c r="J13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>